<commit_message>
opened and closed file. No changes to data
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2019_SteelheadData.xlsx
+++ b/analysis/data/raw_data/2019_SteelheadData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsmsj\Desktop\Primary Work\1. Research\1. Adult Monitoring\2.5 Steelhead Redd Surveys\Data\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C6B38F-1EB6-264A-8A24-5341453A0EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13930" windowHeight="10370"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20780" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Census2019" sheetId="11" r:id="rId1"/>
@@ -19,10 +20,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Census2019!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -523,7 +533,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,7 +663,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -930,21 +940,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="13" width="13.453125" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="8.90625" style="8"/>
+    <col min="1" max="13" width="13.5" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -985,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1077,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1149,7 +1159,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -1190,7 +1200,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1231,7 +1241,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1272,7 +1282,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1313,7 +1323,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1487,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
@@ -1518,7 +1528,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1559,7 +1569,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1610,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
@@ -1641,7 +1651,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1692,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>11</v>
       </c>
@@ -1723,7 +1733,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
         <v>11</v>
       </c>
@@ -1764,7 +1774,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1815,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
         <v>11</v>
       </c>
@@ -1846,7 +1856,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1897,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="8" t="s">
         <v>11</v>
       </c>
@@ -1928,7 +1938,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
         <v>11</v>
       </c>
@@ -1969,7 +1979,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
         <v>11</v>
       </c>
@@ -2010,7 +2020,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
         <v>11</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="8" t="s">
         <v>11</v>
       </c>
@@ -2092,7 +2102,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -2133,7 +2143,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
         <v>11</v>
       </c>
@@ -2174,7 +2184,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
@@ -2215,7 +2225,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="8" t="s">
         <v>11</v>
       </c>
@@ -2256,7 +2266,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
         <v>11</v>
       </c>
@@ -2297,7 +2307,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
         <v>11</v>
       </c>
@@ -2379,7 +2389,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
         <v>11</v>
       </c>
@@ -2420,7 +2430,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37" s="8" t="s">
         <v>11</v>
       </c>
@@ -2461,7 +2471,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>11</v>
       </c>
@@ -2502,7 +2512,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
         <v>11</v>
       </c>
@@ -2543,7 +2553,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40" s="8" t="s">
         <v>11</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
         <v>11</v>
       </c>
@@ -2625,7 +2635,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
         <v>11</v>
       </c>
@@ -2666,7 +2676,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
         <v>11</v>
       </c>
@@ -2707,7 +2717,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
         <v>11</v>
       </c>
@@ -2748,7 +2758,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
         <v>11</v>
       </c>
@@ -2789,7 +2799,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="8" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2840,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
         <v>11</v>
       </c>
@@ -2871,7 +2881,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48" s="8" t="s">
         <v>11</v>
       </c>
@@ -2912,7 +2922,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
         <v>11</v>
       </c>
@@ -2953,7 +2963,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="8" t="s">
         <v>11</v>
       </c>
@@ -2994,7 +3004,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
         <v>11</v>
       </c>
@@ -3035,7 +3045,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="8" t="s">
         <v>11</v>
       </c>
@@ -3076,7 +3086,7 @@
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="8" t="s">
         <v>11</v>
       </c>
@@ -3117,7 +3127,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A54" s="8" t="s">
         <v>11</v>
       </c>
@@ -3158,7 +3168,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
         <v>11</v>
       </c>
@@ -3199,7 +3209,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
         <v>11</v>
       </c>
@@ -3240,7 +3250,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A57" s="8" t="s">
         <v>11</v>
       </c>
@@ -3281,7 +3291,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
         <v>11</v>
       </c>
@@ -3322,7 +3332,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A59" s="8" t="s">
         <v>11</v>
       </c>
@@ -3363,7 +3373,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A60" s="8" t="s">
         <v>11</v>
       </c>
@@ -3404,7 +3414,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A61" s="8" t="s">
         <v>11</v>
       </c>
@@ -3445,7 +3455,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
         <v>11</v>
       </c>
@@ -3486,7 +3496,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63" s="8" t="s">
         <v>25</v>
       </c>
@@ -3527,7 +3537,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A64" s="8" t="s">
         <v>25</v>
       </c>
@@ -3568,7 +3578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="8" t="s">
         <v>25</v>
       </c>
@@ -3609,7 +3619,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A66" s="8" t="s">
         <v>25</v>
       </c>
@@ -3650,7 +3660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A67" s="8" t="s">
         <v>25</v>
       </c>
@@ -3691,7 +3701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A68" s="8" t="s">
         <v>25</v>
       </c>
@@ -3732,7 +3742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69" s="8" t="s">
         <v>25</v>
       </c>
@@ -3773,7 +3783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
         <v>25</v>
       </c>
@@ -3814,7 +3824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71" s="8" t="s">
         <v>119</v>
       </c>
@@ -3855,7 +3865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="8" t="s">
         <v>119</v>
       </c>
@@ -3896,7 +3906,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="8" t="s">
         <v>119</v>
       </c>
@@ -3937,7 +3947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74" s="8" t="s">
         <v>119</v>
       </c>
@@ -3978,7 +3988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A75" s="8" t="s">
         <v>119</v>
       </c>
@@ -4019,7 +4029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A76" s="8" t="s">
         <v>119</v>
       </c>
@@ -4060,7 +4070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="8" t="s">
         <v>119</v>
       </c>
@@ -4101,7 +4111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A78" s="8" t="s">
         <v>119</v>
       </c>
@@ -4142,7 +4152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="8" t="s">
         <v>119</v>
       </c>
@@ -4183,7 +4193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="8" t="s">
         <v>28</v>
       </c>
@@ -4224,7 +4234,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="8" t="s">
         <v>28</v>
       </c>
@@ -4265,7 +4275,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82" s="8" t="s">
         <v>28</v>
       </c>
@@ -4306,7 +4316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="8" t="s">
         <v>28</v>
       </c>
@@ -4347,7 +4357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="8" t="s">
         <v>28</v>
       </c>
@@ -4388,7 +4398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="8" t="s">
         <v>28</v>
       </c>
@@ -4429,7 +4439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="8" t="s">
         <v>28</v>
       </c>
@@ -4470,7 +4480,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="8" t="s">
         <v>28</v>
       </c>
@@ -4511,7 +4521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="8" t="s">
         <v>28</v>
       </c>
@@ -4559,20 +4569,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="11.6328125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="11.6328125" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="9"/>
+    <col min="1" max="4" width="11.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4592,7 +4602,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -4612,7 +4622,7 @@
         <v>403998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -4632,7 +4642,7 @@
         <v>78797</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -4652,7 +4662,7 @@
         <v>979010</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -4672,7 +4682,7 @@
         <v>229542</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -4692,7 +4702,7 @@
         <v>182150.08000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -4712,7 +4722,7 @@
         <v>22391</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -4732,7 +4742,7 @@
         <v>140270.08000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -4752,7 +4762,7 @@
         <v>331242.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -4772,7 +4782,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -4792,7 +4802,7 @@
         <v>241992</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -4812,7 +4822,7 @@
         <v>497756</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -4832,7 +4842,7 @@
         <v>247416</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -4852,7 +4862,7 @@
         <v>909277</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -4872,7 +4882,7 @@
         <v>633704</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -4899,19 +4909,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.81640625" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="4"/>
+    <col min="1" max="1" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="13.83203125" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="18" t="s">
         <v>33</v>
@@ -4938,7 +4948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -4968,7 +4978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>43</v>
       </c>
@@ -4998,7 +5008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -5028,7 +5038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -5058,7 +5068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5069,7 +5079,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5080,7 +5090,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>1</v>
       </c>
@@ -5103,7 +5113,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -5127,7 +5137,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -5151,7 +5161,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -5175,7 +5185,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -5199,7 +5209,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -5223,7 +5233,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
added script to prep the 2021 wenatchee data
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/2019_SteelheadData.xlsx
+++ b/analysis/data/raw_data/2019_SteelheadData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/kevin_see_dfw_wa_gov/Documents/Documents/Git/MyProjects/UCSthdReddObsErr/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C6B38F-1EB6-264A-8A24-5341453A0EEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C7C6B38F-1EB6-264A-8A24-5341453A0EEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{62D0A1EB-9F10-4C26-A6D8-E0D14455B7C0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20780" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Census2019" sheetId="11" r:id="rId1"/>
@@ -943,18 +943,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="13.5" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="8"/>
+    <col min="1" max="13" width="13.453125" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -995,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>11</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>11</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>11</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>11</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>11</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>11</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>11</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>11</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0.55600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>11</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>11</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>11</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>11</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>11</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>11</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>11</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>11</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>11</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>11</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>11</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>11</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>11</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>11</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>11</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>11</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>11</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>11</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>11</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>11</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>11</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="s">
         <v>11</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>11</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>11</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>11</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>11</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>11</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>11</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>11</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="s">
         <v>11</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>11</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="s">
         <v>25</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>25</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="s">
         <v>25</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="s">
         <v>25</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="s">
         <v>25</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>25</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>25</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="s">
         <v>25</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>119</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>119</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>119</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="s">
         <v>119</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="s">
         <v>119</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="s">
         <v>119</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="s">
         <v>119</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="s">
         <v>119</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="s">
         <v>119</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
         <v>28</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="s">
         <v>28</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="s">
         <v>28</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
         <v>28</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="s">
         <v>28</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
         <v>28</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="s">
         <v>28</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="s">
         <v>28</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="s">
         <v>28</v>
       </c>
@@ -4572,17 +4572,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="11.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.6640625" style="9"/>
+    <col min="1" max="4" width="11.6328125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="8.6328125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>403998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>78797</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>979010</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>229542</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>182150.08000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>22391</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>140270.08000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>331242.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -4802,7 +4802,7 @@
         <v>241992</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>497756</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>247416</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>909277</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>633704</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -4914,14 +4914,14 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="13.83203125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="15.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="13.81640625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="18" t="s">
         <v>33</v>
@@ -4948,7 +4948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>43</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>42</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5079,7 +5079,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5090,7 +5090,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="19" t="s">
         <v>1</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -5161,7 +5161,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -5185,7 +5185,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -5209,7 +5209,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -5233,7 +5233,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>155</v>
       </c>

</xml_diff>